<commit_message>
create folder with part of the zip file that are relevant to contruction of objects
</commit_message>
<xml_diff>
--- a/specifications/mainClassification.xlsx
+++ b/specifications/mainClassification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/san256/users_for_mac_system_macPro/jeannerat/mygit/djeanner/ResearchObjectFinder/specifications/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38505E23-E2AA-2348-BDE4-F7D7A66FA23A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{327319DB-ED9D-B545-9E09-63F0545F3AB3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="640" yWindow="460" windowWidth="48840" windowHeight="25020" xr2:uid="{288A7D19-BA45-F740-BC65-6AFB5F080D47}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="156">
   <si>
     <t>TYPEint 0, TYPEstring "SCF Done"</t>
   </si>
@@ -211,9 +211,6 @@
   </si>
   <si>
     <t>1H</t>
-  </si>
-  <si>
-    <t>complement</t>
   </si>
   <si>
     <t>13C</t>
@@ -484,9 +481,6 @@
     <t>STEP1:</t>
   </si>
   <si>
-    <t>.out .log .txt</t>
-  </si>
-  <si>
     <t>Note the starting point to consider an object is always a file. Therefore will go through the list of files in an archiave/file tree</t>
   </si>
   <si>
@@ -505,36 +499,12 @@
     <t>Step 2: Overt the list of Step 1,  test of presence of related files. (to speed up testing,  this walk the folders and store the names of files of parents folder and full current folde before start testing. This imposes to go through the files before the folder when exploring - testing  single string is faster then multiplet - knowing the oder allows to speedup). make a list of related files that needs to be read and the test to make in each of them .</t>
   </si>
   <si>
-    <t>.cdx</t>
-  </si>
-  <si>
-    <t>.cdxml</t>
-  </si>
-  <si>
-    <t>.sdf</t>
-  </si>
-  <si>
-    <t>.mol</t>
-  </si>
-  <si>
-    <t>acqus</t>
-  </si>
-  <si>
-    <t>acqu2s</t>
-  </si>
-  <si>
     <t>TYPEstring "acqus", TYPEint 2, TYPEstring "##$NUC1= &lt;2H&gt;"</t>
   </si>
   <si>
     <t>This allows to filter the list of file to analyse using fileHasFileNameOrExtension()</t>
   </si>
   <si>
-    <t>procs</t>
-  </si>
-  <si>
-    <t>proc2s</t>
-  </si>
-  <si>
     <t>KEYfile Includes</t>
   </si>
   <si>
@@ -571,12 +541,6 @@
     <t>! TYPEstring "acqus", TYPEint 2, TYPEstring "##$dept"</t>
   </si>
   <si>
-    <t>TYPEstring "acqu2s", TYPEint 0</t>
-  </si>
-  <si>
-    <t>TYPEstring "proc2s", TYPEint 0</t>
-  </si>
-  <si>
     <t>! TYPEstring "acqus", TYPEint 2, TYPEstring "inviet"</t>
   </si>
   <si>
@@ -632,6 +596,51 @@
   </si>
   <si>
     <t>2DNMR</t>
+  </si>
+  <si>
+    <t>".out" ".log" ".txt"</t>
+  </si>
+  <si>
+    <t>".cdx"</t>
+  </si>
+  <si>
+    <t>".cdxml"</t>
+  </si>
+  <si>
+    <t>".mol"</t>
+  </si>
+  <si>
+    <t>".sdf"</t>
+  </si>
+  <si>
+    <t>"acqus"</t>
+  </si>
+  <si>
+    <t>"procs"</t>
+  </si>
+  <si>
+    <t>"acqu2s"</t>
+  </si>
+  <si>
+    <t>"proc2s"</t>
+  </si>
+  <si>
+    <t>Copy paste this to word as unformatted text and save from word as unformatted text</t>
+  </si>
+  <si>
+    <t>open/save in editor to restore end of line</t>
+  </si>
+  <si>
+    <t>2D SDF file</t>
+  </si>
+  <si>
+    <t>3D MOL file</t>
+  </si>
+  <si>
+    <t>3D SDF file</t>
+  </si>
+  <si>
+    <t>empty</t>
   </si>
 </sst>
 </file>
@@ -1098,10 +1107,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3CCB2B3-F360-AF4C-9796-0D615AC2EE3F}">
-  <dimension ref="A1:AB76"/>
+  <dimension ref="A1:AB78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="Z10" sqref="Z10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1122,7 +1131,8 @@
     <col min="18" max="18" width="26.33203125" customWidth="1"/>
     <col min="19" max="21" width="22.1640625" customWidth="1"/>
     <col min="22" max="22" width="33.33203125" customWidth="1"/>
-    <col min="24" max="24" width="16" customWidth="1"/>
+    <col min="23" max="23" width="35" customWidth="1"/>
+    <col min="24" max="24" width="8" customWidth="1"/>
     <col min="25" max="25" width="20.1640625" customWidth="1"/>
     <col min="26" max="26" width="24" customWidth="1"/>
     <col min="28" max="28" width="26.1640625" customWidth="1"/>
@@ -1131,339 +1141,330 @@
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C1" t="s">
-        <v>104</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C2" t="s">
-        <v>105</v>
-      </c>
-      <c r="K2" t="s">
-        <v>107</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C3" t="s">
-        <v>108</v>
-      </c>
-      <c r="J3" t="s">
         <v>102</v>
-      </c>
-      <c r="K3" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C4" t="s">
-        <v>109</v>
+        <v>103</v>
+      </c>
+      <c r="K4" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C5" t="s">
         <v>106</v>
       </c>
+      <c r="J5" t="s">
+        <v>101</v>
+      </c>
+      <c r="K5" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C6" t="s">
-        <v>98</v>
-      </c>
-      <c r="P6" t="s">
-        <v>144</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="8" spans="1:27" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="C8" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" t="s">
         <v>97</v>
       </c>
-      <c r="D8" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="O8" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="P8" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q8" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="R8" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="S8" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="V8" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="W8" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="Y8" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:27" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="C9" t="s">
-        <v>98</v>
-      </c>
-      <c r="D9"/>
-      <c r="F9" s="7" t="s">
-        <v>123</v>
+      <c r="P8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:27" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="C10" t="s">
-        <v>117</v>
-      </c>
-      <c r="D10" t="s">
-        <v>122</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="C10" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="O10" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="P10" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="R10" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="S10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="T10" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="U10" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="V10" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="W10" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="X10" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="Y10" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>100</v>
+      </c>
       <c r="C11" t="s">
-        <v>103</v>
-      </c>
-      <c r="D11" t="s">
-        <v>121</v>
-      </c>
-      <c r="O11" t="s">
-        <v>136</v>
-      </c>
-      <c r="P11">
+        <v>97</v>
+      </c>
+      <c r="D11"/>
+      <c r="F11" s="7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C12" t="s">
+        <v>109</v>
+      </c>
+      <c r="D12" t="s">
+        <v>112</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>141</v>
+      </c>
+      <c r="D13" t="s">
+        <v>111</v>
+      </c>
+      <c r="O13" t="s">
+        <v>124</v>
+      </c>
+      <c r="P13">
         <v>100</v>
       </c>
-      <c r="Q11" t="s">
-        <v>13</v>
-      </c>
-      <c r="R11" t="s">
+      <c r="Q13" t="s">
+        <v>13</v>
+      </c>
+      <c r="R13" t="s">
         <v>6</v>
       </c>
-      <c r="S11" t="s">
+      <c r="S13" t="s">
         <v>58</v>
       </c>
-      <c r="Y11" t="s">
+      <c r="Y13" t="s">
         <v>17</v>
       </c>
-      <c r="Z11" t="s">
+      <c r="Z13" t="s">
         <v>16</v>
       </c>
-      <c r="AA11" s="1" t="s">
+      <c r="AA13" s="1" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F12" s="1"/>
-      <c r="P12">
-        <v>10</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>13</v>
-      </c>
-      <c r="R12" t="s">
-        <v>2</v>
-      </c>
-      <c r="S12" t="s">
-        <v>1</v>
-      </c>
-      <c r="V12" s="1"/>
-      <c r="W12" t="s">
-        <v>48</v>
-      </c>
-      <c r="Y12" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="Z12" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="AA12" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F13" s="1"/>
-      <c r="P13">
-        <v>10</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>13</v>
-      </c>
-      <c r="R13" t="s">
-        <v>2</v>
-      </c>
-      <c r="S13" t="s">
-        <v>1</v>
-      </c>
-      <c r="W13" t="s">
-        <v>49</v>
-      </c>
-      <c r="Y13" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F14" s="1"/>
       <c r="P14">
         <v>10</v>
       </c>
+      <c r="Q14" t="s">
+        <v>13</v>
+      </c>
+      <c r="R14" t="s">
+        <v>2</v>
+      </c>
+      <c r="S14" t="s">
+        <v>1</v>
+      </c>
+      <c r="V14" s="1"/>
       <c r="W14" t="s">
-        <v>50</v>
+        <v>48</v>
+      </c>
+      <c r="Y14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA14" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E15" s="2"/>
+        <v>70</v>
+      </c>
       <c r="F15" s="1"/>
       <c r="P15">
         <v>10</v>
       </c>
+      <c r="Q15" t="s">
+        <v>13</v>
+      </c>
+      <c r="R15" t="s">
+        <v>2</v>
+      </c>
+      <c r="S15" t="s">
+        <v>1</v>
+      </c>
       <c r="W15" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="Y15" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E16" s="2"/>
+        <v>70</v>
+      </c>
       <c r="F16" s="1"/>
       <c r="P16">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="W16" t="s">
-        <v>52</v>
-      </c>
-      <c r="Y16" t="s">
-        <v>9</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="C17" t="s">
-        <v>110</v>
+      <c r="A17" s="1" t="s">
+        <v>70</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="1"/>
-      <c r="G17" s="2"/>
-      <c r="O17" t="s">
-        <v>138</v>
-      </c>
       <c r="P17">
         <v>10</v>
       </c>
-      <c r="Q17" t="s">
-        <v>13</v>
-      </c>
-      <c r="R17" t="s">
+      <c r="W17" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E18" s="2"/>
+      <c r="F18" s="1"/>
+      <c r="P18">
+        <v>20</v>
+      </c>
+      <c r="W18" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
+        <v>142</v>
+      </c>
+      <c r="E19" s="2"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="2"/>
+      <c r="O19" t="s">
+        <v>126</v>
+      </c>
+      <c r="P19">
+        <v>10</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>13</v>
+      </c>
+      <c r="R19" t="s">
         <v>6</v>
       </c>
-      <c r="S17" t="s">
+      <c r="S19" t="s">
         <v>8</v>
       </c>
-      <c r="Y17" t="s">
+      <c r="Y19" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="C18" t="s">
-        <v>111</v>
-      </c>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="O18" t="s">
-        <v>137</v>
-      </c>
-      <c r="P18">
-        <v>10</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>13</v>
-      </c>
-      <c r="R18" t="s">
-        <v>6</v>
-      </c>
-      <c r="S18" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>71</v>
-      </c>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.2">
       <c r="C20" t="s">
-        <v>113</v>
+        <v>143</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="O20" t="s">
-        <v>18</v>
+        <v>125</v>
       </c>
       <c r="P20">
         <v>10</v>
@@ -1475,57 +1476,32 @@
         <v>6</v>
       </c>
       <c r="S20" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y20" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Z20" t="s">
-        <v>21</v>
+        <v>8</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="C21" t="s">
-        <v>112</v>
+      <c r="A21" t="s">
+        <v>70</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
-      <c r="O21" t="s">
-        <v>19</v>
-      </c>
-      <c r="P21">
-        <v>10</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>13</v>
-      </c>
-      <c r="R21" t="s">
-        <v>6</v>
-      </c>
-      <c r="S21" t="s">
-        <v>24</v>
-      </c>
-      <c r="Y21" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Z21" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.2">
       <c r="C22" t="s">
-        <v>113</v>
-      </c>
-      <c r="E22" t="s">
-        <v>139</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="O22" t="s">
         <v>18</v>
       </c>
       <c r="P22">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="Q22" t="s">
         <v>13</v>
@@ -1534,10 +1510,7 @@
         <v>6</v>
       </c>
       <c r="S22" t="s">
-        <v>25</v>
-      </c>
-      <c r="W22" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="Y22" s="1" t="s">
         <v>20</v>
@@ -1548,17 +1521,16 @@
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.2">
       <c r="C23" t="s">
-        <v>112</v>
-      </c>
-      <c r="E23" t="s">
-        <v>139</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="O23" t="s">
         <v>19</v>
       </c>
       <c r="P23">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="Q23" t="s">
         <v>13</v>
@@ -1567,10 +1539,7 @@
         <v>6</v>
       </c>
       <c r="S23" t="s">
-        <v>26</v>
-      </c>
-      <c r="W23" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="Y23" s="1" t="s">
         <v>20</v>
@@ -1581,10 +1550,10 @@
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.2">
       <c r="C24" t="s">
-        <v>113</v>
+        <v>144</v>
       </c>
       <c r="E24" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="G24" s="2"/>
       <c r="O24" t="s">
@@ -1600,10 +1569,10 @@
         <v>6</v>
       </c>
       <c r="S24" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="W24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Y24" s="1" t="s">
         <v>20</v>
@@ -1614,14 +1583,14 @@
     </row>
     <row r="25" spans="1:28" x14ac:dyDescent="0.2">
       <c r="C25" t="s">
-        <v>112</v>
+        <v>145</v>
       </c>
       <c r="E25" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="G25" s="2"/>
       <c r="O25" t="s">
-        <v>19</v>
+        <v>152</v>
       </c>
       <c r="P25">
         <v>20</v>
@@ -1633,10 +1602,10 @@
         <v>6</v>
       </c>
       <c r="S25" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="W25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Y25" s="1" t="s">
         <v>20</v>
@@ -1647,14 +1616,14 @@
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.2">
       <c r="C26" t="s">
-        <v>112</v>
+        <v>144</v>
       </c>
       <c r="E26" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="G26" s="2"/>
       <c r="O26" t="s">
-        <v>34</v>
+        <v>153</v>
       </c>
       <c r="P26">
         <v>20</v>
@@ -1663,10 +1632,13 @@
         <v>13</v>
       </c>
       <c r="R26" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="S26" t="s">
-        <v>35</v>
+        <v>27</v>
+      </c>
+      <c r="W26" t="s">
+        <v>46</v>
       </c>
       <c r="Y26" s="1" t="s">
         <v>20</v>
@@ -1674,163 +1646,152 @@
       <c r="Z26" t="s">
         <v>21</v>
       </c>
-      <c r="AA26" t="s">
+    </row>
+    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="C27" t="s">
+        <v>145</v>
+      </c>
+      <c r="E27" t="s">
+        <v>128</v>
+      </c>
+      <c r="G27" s="2"/>
+      <c r="O27" t="s">
+        <v>154</v>
+      </c>
+      <c r="P27">
+        <v>20</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>13</v>
+      </c>
+      <c r="R27" t="s">
+        <v>6</v>
+      </c>
+      <c r="S27" t="s">
+        <v>28</v>
+      </c>
+      <c r="W27" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y27" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z27" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="C28" t="s">
+        <v>145</v>
+      </c>
+      <c r="E28" t="s">
+        <v>129</v>
+      </c>
+      <c r="G28" s="2"/>
+      <c r="O28" t="s">
+        <v>34</v>
+      </c>
+      <c r="P28">
+        <v>20</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>13</v>
+      </c>
+      <c r="R28" t="s">
+        <v>2</v>
+      </c>
+      <c r="S28" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y28" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z28" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA28" t="s">
         <v>36</v>
       </c>
-      <c r="AB26" t="s">
+      <c r="AB28" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>71</v>
-      </c>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="Y27" s="1"/>
-    </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>71</v>
-      </c>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
     </row>
     <row r="29" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>71</v>
-      </c>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="1"/>
-      <c r="O29" s="1"/>
-      <c r="Q29" t="s">
-        <v>13</v>
-      </c>
-      <c r="R29" t="s">
+        <v>70</v>
+      </c>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="Y29" s="1"/>
+    </row>
+    <row r="30" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>70</v>
+      </c>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+    </row>
+    <row r="31" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>70</v>
+      </c>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="1"/>
+      <c r="O31" s="1"/>
+      <c r="Q31" t="s">
+        <v>13</v>
+      </c>
+      <c r="R31" t="s">
         <v>29</v>
       </c>
-      <c r="Y29" s="1" t="s">
+      <c r="Y31" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="Z29" s="1"/>
-    </row>
-    <row r="30" spans="1:28" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
-      <c r="Q30" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="R30" s="7" t="s">
+      <c r="Z31" s="1"/>
+    </row>
+    <row r="32" spans="1:28" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="Q32" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="R32" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="S30" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="T30" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="U30" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="V30" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="W30" s="7" t="s">
+      <c r="S32" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="T32" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="U32" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="V32" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="W32" s="7" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="C31" t="s">
-        <v>114</v>
-      </c>
-      <c r="E31" s="2"/>
-      <c r="F31" t="s">
-        <v>124</v>
-      </c>
-      <c r="O31" t="s">
-        <v>55</v>
-      </c>
-      <c r="P31">
-        <v>10</v>
-      </c>
-      <c r="Q31" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="R31" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="S31" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="T31" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="U31" s="5"/>
-      <c r="W31" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="C32" t="s">
-        <v>118</v>
-      </c>
-      <c r="E32" s="2"/>
-      <c r="F32" t="s">
-        <v>43</v>
-      </c>
-      <c r="G32" t="s">
-        <v>126</v>
-      </c>
-      <c r="H32" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="I32" t="s">
-        <v>129</v>
-      </c>
-      <c r="O32" t="s">
-        <v>56</v>
-      </c>
-      <c r="P32">
-        <v>20</v>
-      </c>
-      <c r="Q32" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="R32" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="S32" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="T32" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="U32" s="5"/>
-      <c r="W32" s="5" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.2">
       <c r="C33" t="s">
-        <v>118</v>
+        <v>146</v>
       </c>
       <c r="E33" s="2"/>
-      <c r="G33" t="s">
-        <v>126</v>
-      </c>
-      <c r="I33" t="s">
-        <v>129</v>
+      <c r="F33" t="s">
+        <v>114</v>
       </c>
       <c r="O33" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="P33">
         <v>10</v>
@@ -1845,35 +1806,32 @@
         <v>40</v>
       </c>
       <c r="T33" s="5" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="U33" s="5"/>
       <c r="W33" s="5" t="s">
-        <v>54</v>
+        <v>92</v>
       </c>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.2">
       <c r="C34" t="s">
-        <v>118</v>
+        <v>147</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" t="s">
         <v>43</v>
       </c>
       <c r="G34" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="I34" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="O34" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="P34">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="Q34" s="5" t="s">
         <v>13</v>
@@ -1885,37 +1843,26 @@
         <v>40</v>
       </c>
       <c r="T34" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="U34" s="5" t="s">
-        <v>61</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="U34" s="5"/>
       <c r="W34" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.2">
       <c r="C35" t="s">
-        <v>118</v>
+        <v>147</v>
       </c>
       <c r="E35" s="2"/>
-      <c r="F35" t="s">
-        <v>43</v>
-      </c>
       <c r="G35" t="s">
-        <v>126</v>
-      </c>
-      <c r="H35" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="I35" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="O35" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="P35">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="Q35" s="5" t="s">
         <v>13</v>
@@ -1927,34 +1874,29 @@
         <v>40</v>
       </c>
       <c r="T35" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="U35" t="s">
-        <v>63</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="U35" s="5"/>
       <c r="W35" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.2">
       <c r="C36" t="s">
-        <v>118</v>
+        <v>147</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" t="s">
         <v>43</v>
       </c>
       <c r="G36" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="I36" t="s">
-        <v>129</v>
+        <v>60</v>
       </c>
       <c r="O36" t="s">
-        <v>92</v>
+        <v>59</v>
       </c>
       <c r="P36">
         <v>30</v>
@@ -1969,10 +1911,10 @@
         <v>40</v>
       </c>
       <c r="T36" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="U36" t="s">
-        <v>63</v>
+        <v>139</v>
+      </c>
+      <c r="U36" s="5" t="s">
+        <v>61</v>
       </c>
       <c r="W36" s="5" t="s">
         <v>54</v>
@@ -1980,23 +1922,20 @@
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.2">
       <c r="C37" t="s">
-        <v>118</v>
+        <v>147</v>
       </c>
       <c r="E37" s="2"/>
       <c r="F37" t="s">
         <v>43</v>
       </c>
       <c r="G37" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="H37" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="I37" t="s">
-        <v>129</v>
+        <v>63</v>
       </c>
       <c r="O37" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="P37">
         <v>30</v>
@@ -2011,10 +1950,10 @@
         <v>40</v>
       </c>
       <c r="T37" s="5" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="U37" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="W37" s="5" t="s">
         <v>54</v>
@@ -2022,23 +1961,20 @@
     </row>
     <row r="38" spans="1:23" x14ac:dyDescent="0.2">
       <c r="C38" t="s">
-        <v>118</v>
+        <v>147</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38" t="s">
         <v>43</v>
       </c>
       <c r="G38" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="H38" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="I38" t="s">
-        <v>129</v>
+        <v>87</v>
       </c>
       <c r="O38" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="P38">
         <v>30</v>
@@ -2053,10 +1989,10 @@
         <v>40</v>
       </c>
       <c r="T38" s="5" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="U38" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="W38" s="5" t="s">
         <v>54</v>
@@ -2064,29 +2000,23 @@
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.2">
       <c r="C39" t="s">
-        <v>118</v>
+        <v>147</v>
       </c>
       <c r="E39" s="2"/>
       <c r="F39" t="s">
         <v>43</v>
       </c>
       <c r="G39" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="I39" t="s">
-        <v>129</v>
-      </c>
-      <c r="J39" t="s">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="O39" t="s">
-        <v>66</v>
+        <v>90</v>
       </c>
       <c r="P39">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="Q39" s="5" t="s">
         <v>13</v>
@@ -2098,10 +2028,10 @@
         <v>40</v>
       </c>
       <c r="T39" s="5" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="U39" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="W39" s="5" t="s">
         <v>54</v>
@@ -2109,29 +2039,23 @@
     </row>
     <row r="40" spans="1:23" x14ac:dyDescent="0.2">
       <c r="C40" t="s">
-        <v>118</v>
+        <v>147</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" t="s">
         <v>43</v>
       </c>
       <c r="G40" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="H40" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="I40" t="s">
-        <v>129</v>
-      </c>
-      <c r="J40" s="10" t="s">
-        <v>131</v>
+        <v>108</v>
       </c>
       <c r="O40" t="s">
-        <v>68</v>
+        <v>89</v>
       </c>
       <c r="P40">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="Q40" s="5" t="s">
         <v>13</v>
@@ -2143,58 +2067,79 @@
         <v>40</v>
       </c>
       <c r="T40" s="5" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="U40" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="W40" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="41" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A41" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B41" s="7"/>
-      <c r="C41" s="7"/>
-      <c r="D41" s="7"/>
+      <c r="C41" t="s">
+        <v>147</v>
+      </c>
       <c r="E41" s="2"/>
-      <c r="H41" s="2"/>
-      <c r="Q41" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="R41" s="7" t="s">
+      <c r="F41" t="s">
+        <v>43</v>
+      </c>
+      <c r="G41" t="s">
+        <v>116</v>
+      </c>
+      <c r="H41" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="J41" t="s">
+        <v>64</v>
+      </c>
+      <c r="O41" t="s">
+        <v>65</v>
+      </c>
+      <c r="P41">
+        <v>40</v>
+      </c>
+      <c r="Q41" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="R41" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="S41" s="7" t="s">
+      <c r="S41" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="T41" s="7"/>
-      <c r="U41" s="7"/>
-      <c r="W41" s="7" t="s">
-        <v>77</v>
+      <c r="T41" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="U41" t="s">
+        <v>62</v>
+      </c>
+      <c r="W41" s="5" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="42" spans="1:23" x14ac:dyDescent="0.2">
       <c r="C42" t="s">
-        <v>115</v>
+        <v>147</v>
       </c>
       <c r="E42" s="2"/>
       <c r="F42" t="s">
-        <v>125</v>
+        <v>43</v>
+      </c>
+      <c r="G42" t="s">
+        <v>116</v>
       </c>
       <c r="H42" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="J42" t="s">
-        <v>132</v>
+        <v>63</v>
+      </c>
+      <c r="J42" s="10" t="s">
+        <v>121</v>
       </c>
       <c r="O42" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="P42">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="Q42" s="5" t="s">
         <v>13</v>
@@ -2206,76 +2151,52 @@
         <v>40</v>
       </c>
       <c r="T42" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="U42" s="5"/>
+        <v>139</v>
+      </c>
+      <c r="U42" t="s">
+        <v>62</v>
+      </c>
       <c r="W42" s="5" t="s">
-        <v>94</v>
+        <v>54</v>
       </c>
     </row>
     <row r="43" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="C43" t="s">
-        <v>119</v>
-      </c>
+      <c r="A43" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B43" s="7"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
       <c r="E43" s="2"/>
-      <c r="F43" t="s">
-        <v>73</v>
-      </c>
-      <c r="G43" t="s">
-        <v>127</v>
-      </c>
-      <c r="H43" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="I43" t="s">
-        <v>129</v>
-      </c>
-      <c r="J43" t="s">
-        <v>72</v>
-      </c>
-      <c r="K43" t="s">
-        <v>133</v>
-      </c>
-      <c r="O43" t="s">
-        <v>75</v>
-      </c>
-      <c r="P43">
-        <v>20</v>
-      </c>
-      <c r="Q43" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="R43" s="5" t="s">
+      <c r="H43" s="2"/>
+      <c r="Q43" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="R43" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="S43" s="5" t="s">
+      <c r="S43" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="T43" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="U43" s="5"/>
-      <c r="W43" s="5" t="s">
-        <v>77</v>
+      <c r="T43" s="7"/>
+      <c r="U43" s="7"/>
+      <c r="W43" s="7" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="44" spans="1:23" x14ac:dyDescent="0.2">
       <c r="C44" t="s">
-        <v>119</v>
+        <v>148</v>
       </c>
       <c r="E44" s="2"/>
-      <c r="G44" t="s">
-        <v>127</v>
-      </c>
-      <c r="H44" s="5"/>
-      <c r="I44" t="s">
-        <v>129</v>
-      </c>
-      <c r="K44" t="s">
-        <v>133</v>
+      <c r="F44" t="s">
+        <v>115</v>
+      </c>
+      <c r="H44" s="5" t="s">
+        <v>120</v>
       </c>
       <c r="O44" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="P44">
         <v>10</v>
@@ -2290,41 +2211,38 @@
         <v>40</v>
       </c>
       <c r="T44" s="5" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="U44" s="5"/>
       <c r="W44" s="5" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
     </row>
     <row r="45" spans="1:23" x14ac:dyDescent="0.2">
       <c r="C45" t="s">
-        <v>119</v>
+        <v>149</v>
       </c>
       <c r="E45" s="2"/>
       <c r="F45" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G45" t="s">
-        <v>127</v>
-      </c>
-      <c r="H45" t="s">
-        <v>60</v>
+        <v>117</v>
+      </c>
+      <c r="H45" s="5" t="s">
+        <v>42</v>
       </c>
       <c r="I45" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="J45" t="s">
-        <v>79</v>
-      </c>
-      <c r="K45" t="s">
-        <v>133</v>
+        <v>71</v>
       </c>
       <c r="O45" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="P45">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="Q45" s="5" t="s">
         <v>13</v>
@@ -2336,46 +2254,30 @@
         <v>40</v>
       </c>
       <c r="T45" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="U45" t="s">
-        <v>61</v>
-      </c>
-      <c r="V45" s="5" t="s">
-        <v>148</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="U45" s="5"/>
       <c r="W45" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="46" spans="1:23" x14ac:dyDescent="0.2">
       <c r="C46" t="s">
+        <v>149</v>
+      </c>
+      <c r="E46" s="2"/>
+      <c r="G46" t="s">
+        <v>117</v>
+      </c>
+      <c r="H46" s="5"/>
+      <c r="I46" t="s">
         <v>119</v>
       </c>
-      <c r="E46" s="2"/>
-      <c r="F46" t="s">
-        <v>73</v>
-      </c>
-      <c r="G46" t="s">
-        <v>127</v>
-      </c>
-      <c r="H46" t="s">
-        <v>60</v>
-      </c>
-      <c r="I46" t="s">
-        <v>129</v>
-      </c>
-      <c r="J46" t="s">
-        <v>79</v>
-      </c>
-      <c r="K46" t="s">
-        <v>133</v>
-      </c>
       <c r="O46" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="P46">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="Q46" s="5" t="s">
         <v>13</v>
@@ -2387,49 +2289,38 @@
         <v>40</v>
       </c>
       <c r="T46" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="U46" t="s">
-        <v>61</v>
-      </c>
-      <c r="V46" s="12" t="s">
-        <v>61</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="U46" s="5"/>
       <c r="W46" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="47" spans="1:23" x14ac:dyDescent="0.2">
       <c r="C47" t="s">
-        <v>119</v>
+        <v>149</v>
       </c>
       <c r="E47" s="2"/>
       <c r="F47" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G47" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="H47" t="s">
         <v>60</v>
       </c>
       <c r="I47" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="J47" t="s">
-        <v>79</v>
-      </c>
-      <c r="K47" t="s">
-        <v>133</v>
-      </c>
-      <c r="L47" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="O47" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="P47">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="Q47" s="5" t="s">
         <v>13</v>
@@ -2441,49 +2332,43 @@
         <v>40</v>
       </c>
       <c r="T47" s="5" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="U47" t="s">
         <v>61</v>
       </c>
-      <c r="V47" s="12" t="s">
-        <v>61</v>
+      <c r="V47" s="5" t="s">
+        <v>136</v>
       </c>
       <c r="W47" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="48" spans="1:23" x14ac:dyDescent="0.2">
       <c r="C48" t="s">
-        <v>119</v>
+        <v>149</v>
       </c>
       <c r="E48" s="2"/>
       <c r="F48" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G48" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="H48" t="s">
         <v>60</v>
       </c>
       <c r="I48" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="J48" t="s">
+        <v>78</v>
+      </c>
+      <c r="O48" t="s">
         <v>79</v>
       </c>
-      <c r="K48" t="s">
-        <v>133</v>
-      </c>
-      <c r="L48" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="O48" t="s">
-        <v>84</v>
-      </c>
       <c r="P48">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="Q48" s="5" t="s">
         <v>13</v>
@@ -2495,7 +2380,7 @@
         <v>40</v>
       </c>
       <c r="T48" s="5" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="U48" t="s">
         <v>61</v>
@@ -2504,37 +2389,37 @@
         <v>61</v>
       </c>
       <c r="W48" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="49" spans="1:23" x14ac:dyDescent="0.2">
       <c r="C49" t="s">
-        <v>119</v>
+        <v>149</v>
       </c>
       <c r="E49" s="2"/>
       <c r="F49" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G49" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="H49" t="s">
         <v>60</v>
       </c>
       <c r="I49" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="J49" t="s">
-        <v>83</v>
-      </c>
-      <c r="K49" t="s">
-        <v>133</v>
+        <v>78</v>
+      </c>
+      <c r="L49" t="s">
+        <v>80</v>
       </c>
       <c r="O49" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="P49">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="Q49" s="5" t="s">
         <v>13</v>
@@ -2546,46 +2431,43 @@
         <v>40</v>
       </c>
       <c r="T49" s="5" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="U49" t="s">
         <v>61</v>
       </c>
-      <c r="V49" s="5" t="s">
-        <v>63</v>
+      <c r="V49" s="12" t="s">
+        <v>61</v>
       </c>
       <c r="W49" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="50" spans="1:23" x14ac:dyDescent="0.2">
       <c r="C50" t="s">
-        <v>119</v>
+        <v>149</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G50" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="H50" t="s">
         <v>60</v>
       </c>
       <c r="I50" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="J50" t="s">
+        <v>78</v>
+      </c>
+      <c r="L50" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="O50" t="s">
         <v>83</v>
-      </c>
-      <c r="K50" t="s">
-        <v>133</v>
-      </c>
-      <c r="L50" t="s">
-        <v>85</v>
-      </c>
-      <c r="O50" t="s">
-        <v>86</v>
       </c>
       <c r="P50">
         <v>50</v>
@@ -2600,49 +2482,43 @@
         <v>40</v>
       </c>
       <c r="T50" s="5" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="U50" t="s">
         <v>61</v>
       </c>
-      <c r="V50" s="5" t="s">
-        <v>63</v>
+      <c r="V50" s="12" t="s">
+        <v>61</v>
       </c>
       <c r="W50" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="51" spans="1:23" x14ac:dyDescent="0.2">
       <c r="C51" t="s">
-        <v>119</v>
+        <v>149</v>
       </c>
       <c r="E51" s="2"/>
       <c r="F51" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G51" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="H51" t="s">
         <v>60</v>
       </c>
       <c r="I51" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="J51" t="s">
-        <v>83</v>
-      </c>
-      <c r="K51" t="s">
-        <v>133</v>
-      </c>
-      <c r="L51" s="10" t="s">
-        <v>134</v>
+        <v>82</v>
       </c>
       <c r="O51" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="P51">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="Q51" s="5" t="s">
         <v>13</v>
@@ -2654,200 +2530,305 @@
         <v>40</v>
       </c>
       <c r="T51" s="5" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="U51" t="s">
         <v>61</v>
       </c>
       <c r="V51" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="W51" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="52" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="C52" t="s">
+        <v>149</v>
+      </c>
       <c r="E52" s="2"/>
-      <c r="Q52" s="5"/>
-      <c r="R52" s="5"/>
-      <c r="S52" s="5"/>
-      <c r="T52" s="5"/>
-      <c r="U52" s="5"/>
-      <c r="W52" s="5"/>
+      <c r="F52" t="s">
+        <v>72</v>
+      </c>
+      <c r="G52" t="s">
+        <v>117</v>
+      </c>
+      <c r="H52" t="s">
+        <v>60</v>
+      </c>
+      <c r="I52" t="s">
+        <v>119</v>
+      </c>
+      <c r="J52" t="s">
+        <v>82</v>
+      </c>
+      <c r="L52" t="s">
+        <v>84</v>
+      </c>
+      <c r="O52" t="s">
+        <v>85</v>
+      </c>
+      <c r="P52">
+        <v>50</v>
+      </c>
+      <c r="Q52" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="R52" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="S52" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="T52" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="U52" t="s">
+        <v>61</v>
+      </c>
+      <c r="V52" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="W52" s="5" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="53" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A53" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="E53" s="3"/>
-      <c r="H53" s="6" t="s">
-        <v>69</v>
+      <c r="C53" t="s">
+        <v>149</v>
+      </c>
+      <c r="E53" s="2"/>
+      <c r="F53" t="s">
+        <v>72</v>
+      </c>
+      <c r="G53" t="s">
+        <v>117</v>
+      </c>
+      <c r="H53" t="s">
+        <v>60</v>
+      </c>
+      <c r="I53" t="s">
+        <v>119</v>
+      </c>
+      <c r="J53" t="s">
+        <v>82</v>
+      </c>
+      <c r="L53" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="O53" t="s">
+        <v>86</v>
+      </c>
+      <c r="P53">
+        <v>50</v>
+      </c>
+      <c r="Q53" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="R53" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="S53" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="T53" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="U53" t="s">
+        <v>61</v>
+      </c>
+      <c r="V53" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="W53" s="5" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="54" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A54" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="H54" s="6" t="s">
-        <v>70</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="E54" s="2"/>
+      <c r="Q54" s="5"/>
+      <c r="R54" s="5"/>
+      <c r="S54" s="5"/>
+      <c r="T54" s="5"/>
+      <c r="U54" s="5"/>
+      <c r="W54" s="5"/>
     </row>
     <row r="55" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A55" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
+      </c>
+      <c r="E55" s="3"/>
+      <c r="H55" s="6" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="56" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A56" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
+      </c>
+      <c r="H56" s="6" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="57" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A57" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="H57" s="11" t="s">
-        <v>145</v>
+        <v>70</v>
       </c>
     </row>
     <row r="58" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A58" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="59" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A59" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
+      </c>
+      <c r="H59" s="11" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="60" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A60" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q60" t="s">
-        <v>14</v>
+        <v>70</v>
       </c>
     </row>
     <row r="61" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A61" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="62" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A62" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
+      </c>
+      <c r="Q62" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="63" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A63" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="R63" s="4" t="s">
-        <v>39</v>
+        <v>70</v>
       </c>
     </row>
     <row r="64" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A64" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="E64" t="s">
-        <v>32</v>
-      </c>
-      <c r="R64" t="s">
-        <v>6</v>
+        <v>70</v>
       </c>
     </row>
     <row r="65" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A65" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="R65" t="s">
-        <v>2</v>
+        <v>70</v>
+      </c>
+      <c r="R65" s="4" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="66" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A66" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
+      </c>
+      <c r="E66" t="s">
+        <v>32</v>
       </c>
       <c r="R66" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A67" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="E67" t="s">
-        <v>96</v>
-      </c>
-      <c r="F67" t="s">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="R67" t="s">
-        <v>29</v>
+        <v>2</v>
       </c>
     </row>
     <row r="68" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A68" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="E68" t="s">
-        <v>95</v>
-      </c>
-      <c r="F68" t="s">
-        <v>47</v>
+        <v>70</v>
+      </c>
+      <c r="R68" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="69" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A69" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>15</v>
+        <v>70</v>
+      </c>
+      <c r="E69" t="s">
+        <v>95</v>
+      </c>
+      <c r="F69" t="s">
+        <v>0</v>
+      </c>
+      <c r="R69" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="70" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A70" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E70" t="s">
-        <v>22</v>
+        <v>94</v>
+      </c>
+      <c r="F70" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="71" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A71" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F71" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
     </row>
     <row r="72" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A72" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
+      </c>
+      <c r="E72" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="73" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A73" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F73" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="74" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A74" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="75" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A75" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="76" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A76" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="77" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A77" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="78" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A78" s="7" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed problems with echo -n
</commit_message>
<xml_diff>
--- a/specifications/mainClassification.xlsx
+++ b/specifications/mainClassification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/san256/users_for_mac_system_macPro/jeannerat/mygit/djeanner/ResearchObjectFinder/specifications/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E8E2F5A-24CF-EB49-BCD4-115EBEE73D51}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F061E08E-7609-3E44-9428-ADF83BE228AE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="640" yWindow="460" windowWidth="48840" windowHeight="25020" xr2:uid="{288A7D19-BA45-F740-BC65-6AFB5F080D47}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{288A7D19-BA45-F740-BC65-6AFB5F080D47}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="156">
   <si>
     <t>TYPEint 0, TYPEstring "SCF Done"</t>
   </si>
@@ -1109,8 +1109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3CCB2B3-F360-AF4C-9796-0D615AC2EE3F}">
   <dimension ref="A1:AB78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="Z10" sqref="Z10"/>
+    <sheetView tabSelected="1" topLeftCell="H20" workbookViewId="0">
+      <selection activeCell="O32" sqref="O32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1760,6 +1760,9 @@
       <c r="E32" s="9"/>
       <c r="F32" s="9"/>
       <c r="G32" s="9"/>
+      <c r="O32" s="7" t="s">
+        <v>131</v>
+      </c>
       <c r="Q32" s="7" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
firsst functional bug to fix...
</commit_message>
<xml_diff>
--- a/specifications/mainClassification.xlsx
+++ b/specifications/mainClassification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/san256/users_for_mac_system_macPro/jeannerat/mygit/djeanner/ResearchObjectFinder/specifications/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F061E08E-7609-3E44-9428-ADF83BE228AE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1EE19B3-B10C-4C44-AAA2-F3C270FF543F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{288A7D19-BA45-F740-BC65-6AFB5F080D47}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="161">
   <si>
     <t>TYPEint 0, TYPEstring "SCF Done"</t>
   </si>
@@ -642,12 +642,27 @@
   <si>
     <t>empty</t>
   </si>
+  <si>
+    <t>Gaussian file with freq calculation</t>
+  </si>
+  <si>
+    <t>Gaussian file with Geom. Optimization</t>
+  </si>
+  <si>
+    <t>Gaussian with NMR shieldings</t>
+  </si>
+  <si>
+    <t>Gaussian with NMR shieldings and J coupling</t>
+  </si>
+  <si>
+    <t>Gaussian with NMR J coupling</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -737,6 +752,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -779,7 +800,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -793,6 +814,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1109,8 +1131,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3CCB2B3-F360-AF4C-9796-0D615AC2EE3F}">
   <dimension ref="A1:AB78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H20" workbookViewId="0">
-      <selection activeCell="O32" sqref="O32"/>
+    <sheetView tabSelected="1" topLeftCell="L6" workbookViewId="0">
+      <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1336,6 +1358,9 @@
         <v>70</v>
       </c>
       <c r="F14" s="1"/>
+      <c r="O14" s="13" t="s">
+        <v>156</v>
+      </c>
       <c r="P14">
         <v>10</v>
       </c>
@@ -1367,6 +1392,9 @@
         <v>70</v>
       </c>
       <c r="F15" s="1"/>
+      <c r="O15" s="13" t="s">
+        <v>157</v>
+      </c>
       <c r="P15">
         <v>10</v>
       </c>
@@ -1391,6 +1419,9 @@
         <v>70</v>
       </c>
       <c r="F16" s="1"/>
+      <c r="O16" s="13" t="s">
+        <v>158</v>
+      </c>
       <c r="P16">
         <v>10</v>
       </c>
@@ -1404,6 +1435,9 @@
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="1"/>
+      <c r="O17" s="13" t="s">
+        <v>160</v>
+      </c>
       <c r="P17">
         <v>10</v>
       </c>
@@ -1420,6 +1454,9 @@
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="1"/>
+      <c r="O18" s="13" t="s">
+        <v>159</v>
+      </c>
       <c r="P18">
         <v>20</v>
       </c>
@@ -2836,5 +2873,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
works using list of files
</commit_message>
<xml_diff>
--- a/specifications/mainClassification.xlsx
+++ b/specifications/mainClassification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/san256/users_for_mac_system_macPro/jeannerat/mygit/djeanner/ResearchObjectFinder/specifications/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1EE19B3-B10C-4C44-AAA2-F3C270FF543F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA239377-1C8F-CF45-BA70-7337F517B42A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{288A7D19-BA45-F740-BC65-6AFB5F080D47}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="162">
   <si>
     <t>TYPEint 0, TYPEstring "SCF Done"</t>
   </si>
@@ -656,6 +656,9 @@
   </si>
   <si>
     <t>Gaussian with NMR J coupling</t>
+  </si>
+  <si>
+    <t>TYPEstring "", TYPEint 0, TYPEstring "SCF Done"</t>
   </si>
 </sst>
 </file>
@@ -1131,8 +1134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3CCB2B3-F360-AF4C-9796-0D615AC2EE3F}">
   <dimension ref="A1:AB78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L6" workbookViewId="0">
-      <selection activeCell="M33" sqref="M33"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1328,6 +1331,9 @@
       <c r="D13" t="s">
         <v>111</v>
       </c>
+      <c r="F13" s="5" t="s">
+        <v>161</v>
+      </c>
       <c r="O13" t="s">
         <v>124</v>
       </c>

</xml_diff>

<commit_message>
better identification of type of NMR spectra
</commit_message>
<xml_diff>
--- a/specifications/mainClassification.xlsx
+++ b/specifications/mainClassification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/san256/users_for_mac_system_macPro/jeannerat/mygit/djeanner/ResearchObjectFinder/specifications/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA239377-1C8F-CF45-BA70-7337F517B42A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86E63CAC-5069-7642-87FE-FBC5F7903933}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{288A7D19-BA45-F740-BC65-6AFB5F080D47}"/>
   </bookViews>
@@ -625,9 +625,6 @@
     <t>"proc2s"</t>
   </si>
   <si>
-    <t>Copy paste this to word as unformatted text and save from word as unformatted text</t>
-  </si>
-  <si>
     <t>open/save in editor to restore end of line</t>
   </si>
   <si>
@@ -659,6 +656,9 @@
   </si>
   <si>
     <t>TYPEstring "", TYPEint 0, TYPEstring "SCF Done"</t>
+  </si>
+  <si>
+    <t>Copy paste this to word as unformatted text and save from word as unformatted text (to avoid excell's export adding double quotes to text fields)</t>
   </si>
 </sst>
 </file>
@@ -1134,8 +1134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3CCB2B3-F360-AF4C-9796-0D615AC2EE3F}">
   <dimension ref="A1:AB78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1169,7 +1169,7 @@
         <v>70</v>
       </c>
       <c r="C1" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.2">
@@ -1177,7 +1177,7 @@
         <v>70</v>
       </c>
       <c r="C2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.2">
@@ -1286,7 +1286,7 @@
         <v>44</v>
       </c>
       <c r="X10" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="Y10" s="7" t="s">
         <v>5</v>
@@ -1332,7 +1332,7 @@
         <v>111</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="O13" t="s">
         <v>124</v>
@@ -1365,7 +1365,7 @@
       </c>
       <c r="F14" s="1"/>
       <c r="O14" s="13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="P14">
         <v>10</v>
@@ -1399,7 +1399,7 @@
       </c>
       <c r="F15" s="1"/>
       <c r="O15" s="13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="P15">
         <v>10</v>
@@ -1426,7 +1426,7 @@
       </c>
       <c r="F16" s="1"/>
       <c r="O16" s="13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="P16">
         <v>10</v>
@@ -1442,7 +1442,7 @@
       <c r="E17" s="2"/>
       <c r="F17" s="1"/>
       <c r="O17" s="13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="P17">
         <v>10</v>
@@ -1461,7 +1461,7 @@
       <c r="E18" s="2"/>
       <c r="F18" s="1"/>
       <c r="O18" s="13" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="P18">
         <v>20</v>
@@ -1633,7 +1633,7 @@
       </c>
       <c r="G25" s="2"/>
       <c r="O25" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="P25">
         <v>20</v>
@@ -1666,7 +1666,7 @@
       </c>
       <c r="G26" s="2"/>
       <c r="O26" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="P26">
         <v>20</v>
@@ -1699,7 +1699,7 @@
       </c>
       <c r="G27" s="2"/>
       <c r="O27" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="P27">
         <v>20</v>

</xml_diff>

<commit_message>
update spcifyer and available functions
</commit_message>
<xml_diff>
--- a/specifications/mainClassification.xlsx
+++ b/specifications/mainClassification.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/san256/users_for_mac_system_macPro/jeannerat/mygit/djeanner/ResearchObjectFinder/specifications/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86E63CAC-5069-7642-87FE-FBC5F7903933}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7736581-C760-2B4D-9A3E-CF8E211F495D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{288A7D19-BA45-F740-BC65-6AFB5F080D47}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="165">
   <si>
     <t>TYPEint 0, TYPEstring "SCF Done"</t>
   </si>
@@ -659,6 +659,15 @@
   </si>
   <si>
     <t>Copy paste this to word as unformatted text and save from word as unformatted text (to avoid excell's export adding double quotes to text fields)</t>
+  </si>
+  <si>
+    <t>19F</t>
+  </si>
+  <si>
+    <t>31P</t>
+  </si>
+  <si>
+    <t>2H</t>
   </si>
 </sst>
 </file>
@@ -1134,8 +1143,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3CCB2B3-F360-AF4C-9796-0D615AC2EE3F}">
   <dimension ref="A1:AB78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+    <sheetView tabSelected="1" topLeftCell="L11" workbookViewId="0">
+      <selection activeCell="U45" sqref="U45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2038,7 +2047,7 @@
         <v>139</v>
       </c>
       <c r="U38" t="s">
-        <v>62</v>
+        <v>162</v>
       </c>
       <c r="W38" s="5" t="s">
         <v>54</v>
@@ -2077,7 +2086,7 @@
         <v>139</v>
       </c>
       <c r="U39" t="s">
-        <v>62</v>
+        <v>163</v>
       </c>
       <c r="W39" s="5" t="s">
         <v>54</v>
@@ -2116,7 +2125,7 @@
         <v>139</v>
       </c>
       <c r="U40" t="s">
-        <v>62</v>
+        <v>164</v>
       </c>
       <c r="W40" s="5" t="s">
         <v>54</v>

</xml_diff>